<commit_message>
Update notes on scenario format
</commit_message>
<xml_diff>
--- a/docs/goals_numbering.xlsx
+++ b/docs/goals_numbering.xlsx
@@ -369,7 +369,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -917,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f>DEC2HEX(B34+C34)</f>
+        <f t="shared" ref="D34:D65" si="2">DEC2HEX(B34+C34)</f>
         <v>74</v>
       </c>
     </row>
@@ -926,14 +929,14 @@
         <v>1</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ref="B35:B98" si="2">116+A35</f>
+        <f t="shared" ref="B35:B98" si="3">116+A35</f>
         <v>117</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f>DEC2HEX(B35+C35)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
     </row>
@@ -942,14 +945,14 @@
         <v>2</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="C36" s="1">
         <v>-4</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f>DEC2HEX(B36+C36)</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
     </row>
@@ -958,14 +961,14 @@
         <v>3</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="C37" s="1">
         <v>-4</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f>DEC2HEX(B37+C37)</f>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
     </row>
@@ -974,14 +977,14 @@
         <v>4</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="str">
-        <f>DEC2HEX(B38+C38)</f>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
     </row>
@@ -990,14 +993,14 @@
         <v>5</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
       </c>
       <c r="D39" s="1" t="str">
-        <f>DEC2HEX(B39+C39)</f>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
     </row>
@@ -1006,14 +1009,14 @@
         <v>6</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="C40" s="1">
         <v>-4</v>
       </c>
       <c r="D40" s="1" t="str">
-        <f>DEC2HEX(B40+C40)</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
@@ -1022,14 +1025,14 @@
         <v>7</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="C41" s="1">
         <v>-4</v>
       </c>
       <c r="D41" s="1" t="str">
-        <f>DEC2HEX(B41+C41)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
     </row>
@@ -1038,14 +1041,14 @@
         <v>8</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
       <c r="D42" s="1" t="str">
-        <f>DEC2HEX(B42+C42)</f>
+        <f t="shared" si="2"/>
         <v>7C</v>
       </c>
     </row>
@@ -1054,14 +1057,14 @@
         <v>9</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="C43" s="1">
         <v>0</v>
       </c>
       <c r="D43" s="1" t="str">
-        <f>DEC2HEX(B43+C43)</f>
+        <f t="shared" si="2"/>
         <v>7D</v>
       </c>
     </row>
@@ -1070,14 +1073,14 @@
         <v>10</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="C44" s="1">
         <v>-4</v>
       </c>
       <c r="D44" s="1" t="str">
-        <f>DEC2HEX(B44+C44)</f>
+        <f t="shared" si="2"/>
         <v>7A</v>
       </c>
     </row>
@@ -1086,14 +1089,14 @@
         <v>11</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="C45" s="1">
         <v>-4</v>
       </c>
       <c r="D45" s="1" t="str">
-        <f>DEC2HEX(B45+C45)</f>
+        <f t="shared" si="2"/>
         <v>7B</v>
       </c>
     </row>
@@ -1102,14 +1105,14 @@
         <v>12</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="C46" s="1">
         <v>0</v>
       </c>
       <c r="D46" s="1" t="str">
-        <f>DEC2HEX(B46+C46)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
     </row>
@@ -1118,14 +1121,14 @@
         <v>13</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" s="1" t="str">
-        <f>DEC2HEX(B47+C47)</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
@@ -1134,14 +1137,14 @@
         <v>14</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="C48" s="1">
         <v>-4</v>
       </c>
       <c r="D48" s="1" t="str">
-        <f>DEC2HEX(B48+C48)</f>
+        <f t="shared" si="2"/>
         <v>7E</v>
       </c>
     </row>
@@ -1150,14 +1153,14 @@
         <v>15</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="C49" s="1">
         <v>-4</v>
       </c>
       <c r="D49" s="1" t="str">
-        <f>DEC2HEX(B49+C49)</f>
+        <f t="shared" si="2"/>
         <v>7F</v>
       </c>
     </row>
@@ -1166,14 +1169,14 @@
         <v>16</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
       </c>
       <c r="D50" s="1" t="str">
-        <f>DEC2HEX(B50+C50)</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
     </row>
@@ -1182,14 +1185,14 @@
         <v>17</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
       </c>
       <c r="D51" s="1" t="str">
-        <f>DEC2HEX(B51+C51)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
@@ -1198,14 +1201,14 @@
         <v>18</v>
       </c>
       <c r="B52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>134</v>
       </c>
       <c r="C52" s="1">
         <v>-4</v>
       </c>
       <c r="D52" s="1" t="str">
-        <f>DEC2HEX(B52+C52)</f>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
     </row>
@@ -1214,14 +1217,14 @@
         <v>19</v>
       </c>
       <c r="B53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="C53" s="1">
         <v>-4</v>
       </c>
       <c r="D53" s="1" t="str">
-        <f>DEC2HEX(B53+C53)</f>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
     </row>
@@ -1230,14 +1233,14 @@
         <v>20</v>
       </c>
       <c r="B54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
       </c>
       <c r="D54" s="1" t="str">
-        <f>DEC2HEX(B54+C54)</f>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
     </row>
@@ -1246,14 +1249,14 @@
         <v>21</v>
       </c>
       <c r="B55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>137</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f>DEC2HEX(B55+C55)</f>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
     </row>
@@ -1262,14 +1265,14 @@
         <v>22</v>
       </c>
       <c r="B56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>138</v>
       </c>
       <c r="C56" s="1">
         <v>-4</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>DEC2HEX(B56+C56)</f>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
     </row>
@@ -1278,14 +1281,14 @@
         <v>23</v>
       </c>
       <c r="B57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>139</v>
       </c>
       <c r="C57" s="1">
         <v>-4</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f>DEC2HEX(B57+C57)</f>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
     </row>
@@ -1294,14 +1297,14 @@
         <v>24</v>
       </c>
       <c r="B58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
       </c>
       <c r="D58" s="1" t="str">
-        <f>DEC2HEX(B58+C58)</f>
+        <f t="shared" si="2"/>
         <v>8C</v>
       </c>
     </row>
@@ -1310,14 +1313,14 @@
         <v>25</v>
       </c>
       <c r="B59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
       </c>
       <c r="D59" s="1" t="str">
-        <f>DEC2HEX(B59+C59)</f>
+        <f t="shared" si="2"/>
         <v>8D</v>
       </c>
     </row>
@@ -1326,14 +1329,14 @@
         <v>26</v>
       </c>
       <c r="B60" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="C60" s="1">
         <v>-4</v>
       </c>
       <c r="D60" s="1" t="str">
-        <f>DEC2HEX(B60+C60)</f>
+        <f t="shared" si="2"/>
         <v>8A</v>
       </c>
     </row>
@@ -1342,14 +1345,14 @@
         <v>27</v>
       </c>
       <c r="B61" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="C61" s="1">
         <v>-4</v>
       </c>
       <c r="D61" s="1" t="str">
-        <f>DEC2HEX(B61+C61)</f>
+        <f t="shared" si="2"/>
         <v>8B</v>
       </c>
     </row>
@@ -1358,14 +1361,14 @@
         <v>28</v>
       </c>
       <c r="B62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>144</v>
       </c>
       <c r="C62" s="1">
         <v>0</v>
       </c>
       <c r="D62" s="1" t="str">
-        <f>DEC2HEX(B62+C62)</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
@@ -1374,14 +1377,14 @@
         <v>29</v>
       </c>
       <c r="B63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="C63" s="1">
         <v>0</v>
       </c>
       <c r="D63" s="1" t="str">
-        <f>DEC2HEX(B63+C63)</f>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
     </row>
@@ -1390,14 +1393,14 @@
         <v>30</v>
       </c>
       <c r="B64" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="C64" s="1">
         <v>-4</v>
       </c>
       <c r="D64" s="1" t="str">
-        <f>DEC2HEX(B64+C64)</f>
+        <f t="shared" si="2"/>
         <v>8E</v>
       </c>
     </row>
@@ -1406,14 +1409,14 @@
         <v>31</v>
       </c>
       <c r="B65" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>147</v>
       </c>
       <c r="C65" s="1">
         <v>-4</v>
       </c>
       <c r="D65" s="1" t="str">
-        <f>DEC2HEX(B65+C65)</f>
+        <f t="shared" si="2"/>
         <v>8F</v>
       </c>
     </row>
@@ -1422,14 +1425,14 @@
         <v>32</v>
       </c>
       <c r="B66" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>148</v>
       </c>
       <c r="C66" s="1">
         <v>0</v>
       </c>
       <c r="D66" s="1" t="str">
-        <f>DEC2HEX(B66+C66)</f>
+        <f t="shared" ref="D66:D97" si="4">DEC2HEX(B66+C66)</f>
         <v>94</v>
       </c>
     </row>
@@ -1438,14 +1441,14 @@
         <v>33</v>
       </c>
       <c r="B67" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>149</v>
       </c>
       <c r="C67" s="1">
         <v>0</v>
       </c>
       <c r="D67" s="1" t="str">
-        <f>DEC2HEX(B67+C67)</f>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
     </row>
@@ -1454,14 +1457,14 @@
         <v>34</v>
       </c>
       <c r="B68" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="C68" s="1">
         <v>-4</v>
       </c>
       <c r="D68" s="1" t="str">
-        <f>DEC2HEX(B68+C68)</f>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
     </row>
@@ -1470,14 +1473,14 @@
         <v>35</v>
       </c>
       <c r="B69" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>151</v>
       </c>
       <c r="C69" s="1">
         <v>-4</v>
       </c>
       <c r="D69" s="1" t="str">
-        <f>DEC2HEX(B69+C69)</f>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
     </row>
@@ -1486,14 +1489,14 @@
         <v>36</v>
       </c>
       <c r="B70" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>152</v>
       </c>
       <c r="C70" s="1">
         <v>0</v>
       </c>
       <c r="D70" s="1" t="str">
-        <f>DEC2HEX(B70+C70)</f>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
     </row>
@@ -1502,14 +1505,14 @@
         <v>37</v>
       </c>
       <c r="B71" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
       <c r="C71" s="1">
         <v>0</v>
       </c>
       <c r="D71" s="1" t="str">
-        <f>DEC2HEX(B71+C71)</f>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
     </row>
@@ -1518,14 +1521,14 @@
         <v>38</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>154</v>
       </c>
       <c r="C72" s="1">
         <v>-4</v>
       </c>
       <c r="D72" s="1" t="str">
-        <f>DEC2HEX(B72+C72)</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
     </row>
@@ -1534,14 +1537,14 @@
         <v>39</v>
       </c>
       <c r="B73" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>155</v>
       </c>
       <c r="C73" s="1">
         <v>-4</v>
       </c>
       <c r="D73" s="1" t="str">
-        <f>DEC2HEX(B73+C73)</f>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
     </row>
@@ -1550,14 +1553,14 @@
         <v>40</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>156</v>
       </c>
       <c r="C74" s="1">
         <v>0</v>
       </c>
       <c r="D74" s="1" t="str">
-        <f>DEC2HEX(B74+C74)</f>
+        <f t="shared" si="4"/>
         <v>9C</v>
       </c>
     </row>
@@ -1566,14 +1569,14 @@
         <v>41</v>
       </c>
       <c r="B75" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
       </c>
       <c r="D75" s="1" t="str">
-        <f>DEC2HEX(B75+C75)</f>
+        <f t="shared" si="4"/>
         <v>9D</v>
       </c>
     </row>
@@ -1582,14 +1585,14 @@
         <v>42</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>158</v>
       </c>
       <c r="C76" s="1">
         <v>-4</v>
       </c>
       <c r="D76" s="1" t="str">
-        <f>DEC2HEX(B76+C76)</f>
+        <f t="shared" si="4"/>
         <v>9A</v>
       </c>
     </row>
@@ -1598,14 +1601,14 @@
         <v>43</v>
       </c>
       <c r="B77" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159</v>
       </c>
       <c r="C77" s="1">
         <v>-4</v>
       </c>
       <c r="D77" s="1" t="str">
-        <f>DEC2HEX(B77+C77)</f>
+        <f t="shared" si="4"/>
         <v>9B</v>
       </c>
     </row>
@@ -1614,14 +1617,14 @@
         <v>44</v>
       </c>
       <c r="B78" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="C78" s="1">
         <v>0</v>
       </c>
       <c r="D78" s="1" t="str">
-        <f>DEC2HEX(B78+C78)</f>
+        <f t="shared" si="4"/>
         <v>A0</v>
       </c>
     </row>
@@ -1630,14 +1633,14 @@
         <v>45</v>
       </c>
       <c r="B79" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>161</v>
       </c>
       <c r="C79" s="1">
         <v>0</v>
       </c>
       <c r="D79" s="1" t="str">
-        <f>DEC2HEX(B79+C79)</f>
+        <f t="shared" si="4"/>
         <v>A1</v>
       </c>
     </row>
@@ -1646,14 +1649,14 @@
         <v>46</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>162</v>
       </c>
       <c r="C80" s="1">
         <v>-4</v>
       </c>
       <c r="D80" s="1" t="str">
-        <f>DEC2HEX(B80+C80)</f>
+        <f t="shared" si="4"/>
         <v>9E</v>
       </c>
     </row>
@@ -1662,14 +1665,14 @@
         <v>47</v>
       </c>
       <c r="B81" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>163</v>
       </c>
       <c r="C81" s="1">
         <v>-4</v>
       </c>
       <c r="D81" s="1" t="str">
-        <f>DEC2HEX(B81+C81)</f>
+        <f t="shared" si="4"/>
         <v>9F</v>
       </c>
     </row>
@@ -1678,14 +1681,14 @@
         <v>48</v>
       </c>
       <c r="B82" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>164</v>
       </c>
       <c r="C82" s="1">
         <v>0</v>
       </c>
       <c r="D82" s="1" t="str">
-        <f>DEC2HEX(B82+C82)</f>
+        <f t="shared" si="4"/>
         <v>A4</v>
       </c>
     </row>
@@ -1694,14 +1697,14 @@
         <v>49</v>
       </c>
       <c r="B83" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>165</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
       </c>
       <c r="D83" s="1" t="str">
-        <f>DEC2HEX(B83+C83)</f>
+        <f t="shared" si="4"/>
         <v>A5</v>
       </c>
     </row>
@@ -1710,14 +1713,14 @@
         <v>50</v>
       </c>
       <c r="B84" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166</v>
       </c>
       <c r="C84" s="1">
         <v>-4</v>
       </c>
       <c r="D84" s="1" t="str">
-        <f>DEC2HEX(B84+C84)</f>
+        <f t="shared" si="4"/>
         <v>A2</v>
       </c>
     </row>
@@ -1726,14 +1729,14 @@
         <v>51</v>
       </c>
       <c r="B85" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>167</v>
       </c>
       <c r="C85" s="1">
         <v>-4</v>
       </c>
       <c r="D85" s="1" t="str">
-        <f>DEC2HEX(B85+C85)</f>
+        <f t="shared" si="4"/>
         <v>A3</v>
       </c>
     </row>
@@ -1742,14 +1745,14 @@
         <v>52</v>
       </c>
       <c r="B86" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>168</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
       </c>
       <c r="D86" s="1" t="str">
-        <f>DEC2HEX(B86+C86)</f>
+        <f t="shared" si="4"/>
         <v>A8</v>
       </c>
     </row>
@@ -1758,14 +1761,14 @@
         <v>53</v>
       </c>
       <c r="B87" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="C87" s="1">
         <v>0</v>
       </c>
       <c r="D87" s="1" t="str">
-        <f>DEC2HEX(B87+C87)</f>
+        <f t="shared" si="4"/>
         <v>A9</v>
       </c>
     </row>
@@ -1774,14 +1777,14 @@
         <v>54</v>
       </c>
       <c r="B88" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
       <c r="C88" s="1">
         <v>-4</v>
       </c>
       <c r="D88" s="1" t="str">
-        <f>DEC2HEX(B88+C88)</f>
+        <f t="shared" si="4"/>
         <v>A6</v>
       </c>
     </row>
@@ -1790,14 +1793,14 @@
         <v>55</v>
       </c>
       <c r="B89" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>171</v>
       </c>
       <c r="C89" s="1">
         <v>-4</v>
       </c>
       <c r="D89" s="1" t="str">
-        <f>DEC2HEX(B89+C89)</f>
+        <f t="shared" si="4"/>
         <v>A7</v>
       </c>
     </row>
@@ -1806,14 +1809,14 @@
         <v>56</v>
       </c>
       <c r="B90" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>172</v>
       </c>
       <c r="C90" s="1">
         <v>0</v>
       </c>
       <c r="D90" s="1" t="str">
-        <f>DEC2HEX(B90+C90)</f>
+        <f t="shared" si="4"/>
         <v>AC</v>
       </c>
     </row>
@@ -1822,14 +1825,14 @@
         <v>57</v>
       </c>
       <c r="B91" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>173</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
       </c>
       <c r="D91" s="1" t="str">
-        <f>DEC2HEX(B91+C91)</f>
+        <f t="shared" si="4"/>
         <v>AD</v>
       </c>
     </row>
@@ -1838,14 +1841,14 @@
         <v>58</v>
       </c>
       <c r="B92" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>174</v>
       </c>
       <c r="C92" s="1">
         <v>-4</v>
       </c>
       <c r="D92" s="1" t="str">
-        <f>DEC2HEX(B92+C92)</f>
+        <f t="shared" si="4"/>
         <v>AA</v>
       </c>
     </row>
@@ -1854,14 +1857,14 @@
         <v>59</v>
       </c>
       <c r="B93" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>175</v>
       </c>
       <c r="C93" s="1">
         <v>-4</v>
       </c>
       <c r="D93" s="1" t="str">
-        <f>DEC2HEX(B93+C93)</f>
+        <f t="shared" si="4"/>
         <v>AB</v>
       </c>
     </row>
@@ -1870,14 +1873,14 @@
         <v>60</v>
       </c>
       <c r="B94" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>176</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
       </c>
       <c r="D94" s="1" t="str">
-        <f>DEC2HEX(B94+C94)</f>
+        <f t="shared" si="4"/>
         <v>B0</v>
       </c>
     </row>
@@ -1886,14 +1889,14 @@
         <v>61</v>
       </c>
       <c r="B95" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>177</v>
       </c>
       <c r="C95" s="1">
         <v>0</v>
       </c>
       <c r="D95" s="1" t="str">
-        <f>DEC2HEX(B95+C95)</f>
+        <f t="shared" si="4"/>
         <v>B1</v>
       </c>
     </row>
@@ -1902,14 +1905,14 @@
         <v>62</v>
       </c>
       <c r="B96" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="C96" s="1">
         <v>-4</v>
       </c>
       <c r="D96" s="1" t="str">
-        <f>DEC2HEX(B96+C96)</f>
+        <f t="shared" si="4"/>
         <v>AE</v>
       </c>
     </row>
@@ -1918,14 +1921,14 @@
         <v>63</v>
       </c>
       <c r="B97" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>179</v>
       </c>
       <c r="C97" s="1">
         <v>-4</v>
       </c>
       <c r="D97" s="1" t="str">
-        <f>DEC2HEX(B97+C97)</f>
+        <f t="shared" si="4"/>
         <v>AF</v>
       </c>
     </row>
@@ -1934,14 +1937,14 @@
         <v>64</v>
       </c>
       <c r="B98" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="D98" s="1" t="str">
-        <f>DEC2HEX(B98+C98)</f>
+        <f t="shared" ref="D98:D129" si="5">DEC2HEX(B98+C98)</f>
         <v>B4</v>
       </c>
     </row>
@@ -1950,14 +1953,14 @@
         <v>65</v>
       </c>
       <c r="B99" s="1">
-        <f t="shared" ref="B99:B133" si="3">116+A99</f>
+        <f t="shared" ref="B99:B133" si="6">116+A99</f>
         <v>181</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
       </c>
       <c r="D99" s="1" t="str">
-        <f>DEC2HEX(B99+C99)</f>
+        <f t="shared" si="5"/>
         <v>B5</v>
       </c>
     </row>
@@ -1966,14 +1969,14 @@
         <v>66</v>
       </c>
       <c r="B100" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>182</v>
       </c>
       <c r="C100" s="1">
         <v>-4</v>
       </c>
       <c r="D100" s="1" t="str">
-        <f>DEC2HEX(B100+C100)</f>
+        <f t="shared" si="5"/>
         <v>B2</v>
       </c>
     </row>
@@ -1982,14 +1985,14 @@
         <v>67</v>
       </c>
       <c r="B101" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>183</v>
       </c>
       <c r="C101" s="1">
         <v>-4</v>
       </c>
       <c r="D101" s="1" t="str">
-        <f>DEC2HEX(B101+C101)</f>
+        <f t="shared" si="5"/>
         <v>B3</v>
       </c>
     </row>
@@ -1998,14 +2001,14 @@
         <v>68</v>
       </c>
       <c r="B102" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>184</v>
       </c>
       <c r="C102" s="1">
         <v>0</v>
       </c>
       <c r="D102" s="1" t="str">
-        <f>DEC2HEX(B102+C102)</f>
+        <f t="shared" si="5"/>
         <v>B8</v>
       </c>
     </row>
@@ -2014,14 +2017,14 @@
         <v>69</v>
       </c>
       <c r="B103" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>185</v>
       </c>
       <c r="C103" s="1">
         <v>0</v>
       </c>
       <c r="D103" s="1" t="str">
-        <f>DEC2HEX(B103+C103)</f>
+        <f t="shared" si="5"/>
         <v>B9</v>
       </c>
     </row>
@@ -2030,14 +2033,14 @@
         <v>70</v>
       </c>
       <c r="B104" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>186</v>
       </c>
       <c r="C104" s="1">
         <v>-4</v>
       </c>
       <c r="D104" s="1" t="str">
-        <f>DEC2HEX(B104+C104)</f>
+        <f t="shared" si="5"/>
         <v>B6</v>
       </c>
     </row>
@@ -2046,14 +2049,14 @@
         <v>71</v>
       </c>
       <c r="B105" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="C105" s="1">
         <v>-4</v>
       </c>
       <c r="D105" s="1" t="str">
-        <f>DEC2HEX(B105+C105)</f>
+        <f t="shared" si="5"/>
         <v>B7</v>
       </c>
     </row>
@@ -2062,14 +2065,14 @@
         <v>72</v>
       </c>
       <c r="B106" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>188</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
       </c>
       <c r="D106" s="1" t="str">
-        <f>DEC2HEX(B106+C106)</f>
+        <f t="shared" si="5"/>
         <v>BC</v>
       </c>
     </row>
@@ -2078,14 +2081,14 @@
         <v>73</v>
       </c>
       <c r="B107" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>189</v>
       </c>
       <c r="C107" s="1">
         <v>0</v>
       </c>
       <c r="D107" s="1" t="str">
-        <f>DEC2HEX(B107+C107)</f>
+        <f t="shared" si="5"/>
         <v>BD</v>
       </c>
     </row>
@@ -2094,14 +2097,14 @@
         <v>74</v>
       </c>
       <c r="B108" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
       <c r="C108" s="1">
         <v>-4</v>
       </c>
       <c r="D108" s="1" t="str">
-        <f>DEC2HEX(B108+C108)</f>
+        <f t="shared" si="5"/>
         <v>BA</v>
       </c>
     </row>
@@ -2110,14 +2113,14 @@
         <v>75</v>
       </c>
       <c r="B109" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>191</v>
       </c>
       <c r="C109" s="1">
         <v>-4</v>
       </c>
       <c r="D109" s="1" t="str">
-        <f>DEC2HEX(B109+C109)</f>
+        <f t="shared" si="5"/>
         <v>BB</v>
       </c>
     </row>
@@ -2126,14 +2129,14 @@
         <v>76</v>
       </c>
       <c r="B110" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C110" s="1">
         <v>0</v>
       </c>
       <c r="D110" s="1" t="str">
-        <f>DEC2HEX(B110+C110)</f>
+        <f t="shared" si="5"/>
         <v>C0</v>
       </c>
     </row>
@@ -2142,14 +2145,14 @@
         <v>77</v>
       </c>
       <c r="B111" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>193</v>
       </c>
       <c r="C111" s="1">
         <v>0</v>
       </c>
       <c r="D111" s="1" t="str">
-        <f>DEC2HEX(B111+C111)</f>
+        <f t="shared" si="5"/>
         <v>C1</v>
       </c>
     </row>
@@ -2158,14 +2161,14 @@
         <v>78</v>
       </c>
       <c r="B112" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>194</v>
       </c>
       <c r="C112" s="1">
         <v>-4</v>
       </c>
       <c r="D112" s="1" t="str">
-        <f>DEC2HEX(B112+C112)</f>
+        <f t="shared" si="5"/>
         <v>BE</v>
       </c>
     </row>
@@ -2174,14 +2177,14 @@
         <v>79</v>
       </c>
       <c r="B113" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>195</v>
       </c>
       <c r="C113" s="1">
         <v>-4</v>
       </c>
       <c r="D113" s="1" t="str">
-        <f>DEC2HEX(B113+C113)</f>
+        <f t="shared" si="5"/>
         <v>BF</v>
       </c>
     </row>
@@ -2190,14 +2193,14 @@
         <v>80</v>
       </c>
       <c r="B114" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>196</v>
       </c>
       <c r="C114" s="1">
         <v>0</v>
       </c>
       <c r="D114" s="1" t="str">
-        <f>DEC2HEX(B114+C114)</f>
+        <f t="shared" si="5"/>
         <v>C4</v>
       </c>
     </row>
@@ -2206,14 +2209,14 @@
         <v>81</v>
       </c>
       <c r="B115" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>197</v>
       </c>
       <c r="C115" s="1">
         <v>0</v>
       </c>
       <c r="D115" s="1" t="str">
-        <f>DEC2HEX(B115+C115)</f>
+        <f t="shared" si="5"/>
         <v>C5</v>
       </c>
     </row>
@@ -2222,14 +2225,14 @@
         <v>82</v>
       </c>
       <c r="B116" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>198</v>
       </c>
       <c r="C116" s="1">
         <v>-4</v>
       </c>
       <c r="D116" s="1" t="str">
-        <f>DEC2HEX(B116+C116)</f>
+        <f t="shared" si="5"/>
         <v>C2</v>
       </c>
     </row>
@@ -2238,14 +2241,14 @@
         <v>83</v>
       </c>
       <c r="B117" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>199</v>
       </c>
       <c r="C117" s="1">
         <v>-4</v>
       </c>
       <c r="D117" s="1" t="str">
-        <f>DEC2HEX(B117+C117)</f>
+        <f t="shared" si="5"/>
         <v>C3</v>
       </c>
     </row>
@@ -2254,14 +2257,14 @@
         <v>84</v>
       </c>
       <c r="B118" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="C118" s="1">
         <v>0</v>
       </c>
       <c r="D118" s="1" t="str">
-        <f>DEC2HEX(B118+C118)</f>
+        <f t="shared" si="5"/>
         <v>C8</v>
       </c>
     </row>
@@ -2270,14 +2273,14 @@
         <v>85</v>
       </c>
       <c r="B119" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>201</v>
       </c>
       <c r="C119" s="1">
         <v>0</v>
       </c>
       <c r="D119" s="1" t="str">
-        <f>DEC2HEX(B119+C119)</f>
+        <f t="shared" si="5"/>
         <v>C9</v>
       </c>
     </row>
@@ -2286,14 +2289,14 @@
         <v>86</v>
       </c>
       <c r="B120" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>202</v>
       </c>
       <c r="C120" s="1">
         <v>-4</v>
       </c>
       <c r="D120" s="1" t="str">
-        <f>DEC2HEX(B120+C120)</f>
+        <f t="shared" si="5"/>
         <v>C6</v>
       </c>
     </row>
@@ -2302,14 +2305,14 @@
         <v>87</v>
       </c>
       <c r="B121" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>203</v>
       </c>
       <c r="C121" s="1">
         <v>-4</v>
       </c>
       <c r="D121" s="1" t="str">
-        <f>DEC2HEX(B121+C121)</f>
+        <f t="shared" si="5"/>
         <v>C7</v>
       </c>
     </row>
@@ -2318,14 +2321,14 @@
         <v>88</v>
       </c>
       <c r="B122" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>204</v>
       </c>
       <c r="C122" s="1">
         <v>0</v>
       </c>
       <c r="D122" s="1" t="str">
-        <f>DEC2HEX(B122+C122)</f>
+        <f t="shared" si="5"/>
         <v>CC</v>
       </c>
     </row>
@@ -2334,14 +2337,14 @@
         <v>89</v>
       </c>
       <c r="B123" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>205</v>
       </c>
       <c r="C123" s="1">
         <v>0</v>
       </c>
       <c r="D123" s="1" t="str">
-        <f>DEC2HEX(B123+C123)</f>
+        <f t="shared" si="5"/>
         <v>CD</v>
       </c>
     </row>
@@ -2350,14 +2353,14 @@
         <v>90</v>
       </c>
       <c r="B124" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>206</v>
       </c>
       <c r="C124" s="1">
         <v>-4</v>
       </c>
       <c r="D124" s="1" t="str">
-        <f>DEC2HEX(B124+C124)</f>
+        <f t="shared" si="5"/>
         <v>CA</v>
       </c>
     </row>
@@ -2366,14 +2369,14 @@
         <v>91</v>
       </c>
       <c r="B125" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>207</v>
       </c>
       <c r="C125" s="1">
         <v>-4</v>
       </c>
       <c r="D125" s="1" t="str">
-        <f>DEC2HEX(B125+C125)</f>
+        <f t="shared" si="5"/>
         <v>CB</v>
       </c>
     </row>
@@ -2382,14 +2385,14 @@
         <v>92</v>
       </c>
       <c r="B126" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>208</v>
       </c>
       <c r="C126" s="1">
         <v>0</v>
       </c>
       <c r="D126" s="1" t="str">
-        <f>DEC2HEX(B126+C126)</f>
+        <f t="shared" si="5"/>
         <v>D0</v>
       </c>
     </row>
@@ -2398,14 +2401,14 @@
         <v>93</v>
       </c>
       <c r="B127" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>209</v>
       </c>
       <c r="C127" s="1">
         <v>0</v>
       </c>
       <c r="D127" s="1" t="str">
-        <f>DEC2HEX(B127+C127)</f>
+        <f t="shared" si="5"/>
         <v>D1</v>
       </c>
     </row>
@@ -2414,14 +2417,14 @@
         <v>94</v>
       </c>
       <c r="B128" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="C128" s="1">
         <v>-4</v>
       </c>
       <c r="D128" s="1" t="str">
-        <f>DEC2HEX(B128+C128)</f>
+        <f t="shared" si="5"/>
         <v>CE</v>
       </c>
     </row>
@@ -2430,14 +2433,14 @@
         <v>95</v>
       </c>
       <c r="B129" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>211</v>
       </c>
       <c r="C129" s="1">
         <v>-4</v>
       </c>
       <c r="D129" s="1" t="str">
-        <f>DEC2HEX(B129+C129)</f>
+        <f t="shared" si="5"/>
         <v>CF</v>
       </c>
     </row>
@@ -2446,14 +2449,14 @@
         <v>96</v>
       </c>
       <c r="B130" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>212</v>
       </c>
       <c r="C130" s="1">
         <v>0</v>
       </c>
       <c r="D130" s="1" t="str">
-        <f>DEC2HEX(B130+C130)</f>
+        <f t="shared" ref="D130:D161" si="7">DEC2HEX(B130+C130)</f>
         <v>D4</v>
       </c>
     </row>
@@ -2462,14 +2465,14 @@
         <v>97</v>
       </c>
       <c r="B131" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>213</v>
       </c>
       <c r="C131" s="1">
         <v>0</v>
       </c>
       <c r="D131" s="1" t="str">
-        <f>DEC2HEX(B131+C131)</f>
+        <f t="shared" si="7"/>
         <v>D5</v>
       </c>
     </row>
@@ -2478,14 +2481,14 @@
         <v>98</v>
       </c>
       <c r="B132" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
       <c r="C132" s="1">
         <v>-4</v>
       </c>
       <c r="D132" s="1" t="str">
-        <f>DEC2HEX(B132+C132)</f>
+        <f t="shared" si="7"/>
         <v>D2</v>
       </c>
     </row>
@@ -2494,14 +2497,14 @@
         <v>99</v>
       </c>
       <c r="B133" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>215</v>
       </c>
       <c r="C133" s="1">
         <v>-4</v>
       </c>
       <c r="D133" s="1" t="str">
-        <f>DEC2HEX(B133+C133)</f>
+        <f t="shared" si="7"/>
         <v>D3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parse traps and scenario goals
</commit_message>
<xml_diff>
--- a/docs/goals_numbering.xlsx
+++ b/docs/goals_numbering.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>VALUE</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>BASE</t>
+  </si>
+  <si>
+    <t>BINARY</t>
+  </si>
+  <si>
+    <t>&amp;</t>
   </si>
 </sst>
 </file>
@@ -367,22 +373,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -390,13 +398,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>-32</v>
       </c>
@@ -404,15 +418,24 @@
         <f t="shared" ref="B2:B33" si="0">116+A2</f>
         <v>84</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2:D33" si="1">DEC2HEX(B2+C2)</f>
+      <c r="C2" s="1" t="str">
+        <f>DEC2BIN(B2)</f>
+        <v>1010100</v>
+      </c>
+      <c r="D2" s="1">
+        <f>_xlfn.BITAND(C2, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2*-2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f t="shared" ref="F2:F33" si="1">DEC2HEX(B2+E2)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>-31</v>
       </c>
@@ -420,15 +443,24 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="str">
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C66" si="2">DEC2BIN(B3)</f>
+        <v>1010101</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D66" si="3">_xlfn.BITAND(C3, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E66" si="4">D3*-2</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="str">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>-30</v>
       </c>
@@ -436,15 +468,24 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="C4" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D4" s="1" t="str">
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1010110</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F4" s="1" t="str">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>-29</v>
       </c>
@@ -452,15 +493,24 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="C5" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D5" s="1" t="str">
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1010111</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>-28</v>
       </c>
@@ -468,15 +518,24 @@
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="str">
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011000</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>-27</v>
       </c>
@@ -484,15 +543,24 @@
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="str">
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011001</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>-26</v>
       </c>
@@ -500,15 +568,24 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="C8" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D8" s="1" t="str">
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011010</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>-25</v>
       </c>
@@ -516,15 +593,24 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="C9" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D9" s="1" t="str">
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011011</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>-24</v>
       </c>
@@ -532,15 +618,24 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="str">
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011100</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>5C</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>-23</v>
       </c>
@@ -548,15 +643,24 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="str">
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011101</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>5D</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>-22</v>
       </c>
@@ -564,15 +668,24 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="C12" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D12" s="1" t="str">
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011110</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>5A</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>-21</v>
       </c>
@@ -580,15 +693,24 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="C13" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D13" s="1" t="str">
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1011111</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>5B</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>-20</v>
       </c>
@@ -596,15 +718,24 @@
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="str">
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100000</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>-19</v>
       </c>
@@ -612,15 +743,24 @@
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="str">
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100001</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>-18</v>
       </c>
@@ -628,15 +768,24 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="C16" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D16" s="1" t="str">
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100010</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>5E</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>-17</v>
       </c>
@@ -644,15 +793,24 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="C17" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D17" s="1" t="str">
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100011</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>5F</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>-16</v>
       </c>
@@ -660,15 +818,24 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="str">
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100100</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>-15</v>
       </c>
@@ -676,15 +843,24 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="str">
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100101</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>-14</v>
       </c>
@@ -692,15 +868,24 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="C20" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D20" s="1" t="str">
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100110</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>-13</v>
       </c>
@@ -708,15 +893,24 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="C21" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D21" s="1" t="str">
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1100111</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>-12</v>
       </c>
@@ -724,15 +918,24 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="str">
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101000</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>-11</v>
       </c>
@@ -740,15 +943,24 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="str">
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101001</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>-10</v>
       </c>
@@ -756,15 +968,24 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="C24" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D24" s="1" t="str">
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101010</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>-9</v>
       </c>
@@ -772,15 +993,24 @@
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="C25" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D25" s="1" t="str">
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101011</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>-8</v>
       </c>
@@ -788,15 +1018,24 @@
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="str">
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101100</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="str">
         <f t="shared" si="1"/>
         <v>6C</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>-7</v>
       </c>
@@ -804,15 +1043,24 @@
         <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="str">
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101101</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="str">
         <f t="shared" si="1"/>
         <v>6D</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>-6</v>
       </c>
@@ -820,15 +1068,24 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="C28" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D28" s="1" t="str">
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101110</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F28" s="1" t="str">
         <f t="shared" si="1"/>
         <v>6A</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>-5</v>
       </c>
@@ -836,15 +1093,24 @@
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="C29" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D29" s="1" t="str">
+      <c r="C29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1101111</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F29" s="1" t="str">
         <f t="shared" si="1"/>
         <v>6B</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>-4</v>
       </c>
@@ -852,15 +1118,24 @@
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="str">
+      <c r="C30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110000</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="str">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>-3</v>
       </c>
@@ -868,15 +1143,24 @@
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1" t="str">
+      <c r="C31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110001</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="str">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>-2</v>
       </c>
@@ -884,15 +1168,24 @@
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="C32" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D32" s="1" t="str">
+      <c r="C32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110010</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F32" s="1" t="str">
         <f t="shared" si="1"/>
         <v>6E</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>-1</v>
       </c>
@@ -900,15 +1193,24 @@
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="C33" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D33" s="1" t="str">
+      <c r="C33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110011</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F33" s="1" t="str">
         <f t="shared" si="1"/>
         <v>6F</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -916,1600 +1218,2500 @@
         <f>116+A34</f>
         <v>116</v>
       </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="str">
-        <f t="shared" ref="D34:D65" si="2">DEC2HEX(B34+C34)</f>
+      <c r="C34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110100</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f>DEC2HEX(B34+E34)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ref="B35:B98" si="3">116+A35</f>
+        <f t="shared" ref="B35:B98" si="5">116+A35</f>
         <v>117</v>
       </c>
-      <c r="C35" s="1">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110101</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f>DEC2HEX(B35+E35)</f>
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="C36" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D36" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110110</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f>DEC2HEX(B36+E36)</f>
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>3</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>119</v>
       </c>
-      <c r="C37" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D37" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1110111</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f>DEC2HEX(B37+E37)</f>
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>4</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111000</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <f>DEC2HEX(B38+E38)</f>
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>5</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>121</v>
       </c>
-      <c r="C39" s="1">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111001</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f>DEC2HEX(B39+E39)</f>
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>6</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>122</v>
       </c>
-      <c r="C40" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D40" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111010</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f>DEC2HEX(B40+E40)</f>
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>7</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>123</v>
       </c>
-      <c r="C41" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D41" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111011</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <f>DEC2HEX(B41+E41)</f>
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>8</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>124</v>
       </c>
-      <c r="C42" s="1">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111100</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <f>DEC2HEX(B42+E42)</f>
         <v>7C</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>9</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C43" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111101</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="str">
+        <f>DEC2HEX(B43+E43)</f>
         <v>7D</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>10</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>126</v>
       </c>
-      <c r="C44" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D44" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C44" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111110</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F44" s="1" t="str">
+        <f>DEC2HEX(B44+E44)</f>
         <v>7A</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>11</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>127</v>
       </c>
-      <c r="C45" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D45" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C45" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1111111</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F45" s="1" t="str">
+        <f>DEC2HEX(B45+E45)</f>
         <v>7B</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>12</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="C46" s="1">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C46" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000000</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="1" t="str">
+        <f>DEC2HEX(B46+E46)</f>
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>13</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>129</v>
       </c>
-      <c r="C47" s="1">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C47" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000001</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="1" t="str">
+        <f>DEC2HEX(B47+E47)</f>
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>14</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>130</v>
       </c>
-      <c r="C48" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D48" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C48" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000010</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F48" s="1" t="str">
+        <f>DEC2HEX(B48+E48)</f>
         <v>7E</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>15</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>131</v>
       </c>
-      <c r="C49" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D49" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C49" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000011</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F49" s="1" t="str">
+        <f>DEC2HEX(B49+E49)</f>
         <v>7F</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>16</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>132</v>
       </c>
-      <c r="C50" s="1">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C50" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000100</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1" t="str">
+        <f>DEC2HEX(B50+E50)</f>
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>17</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>133</v>
       </c>
-      <c r="C51" s="1">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C51" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000101</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1" t="str">
+        <f>DEC2HEX(B51+E51)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>18</v>
       </c>
       <c r="B52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
-      <c r="C52" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D52" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C52" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000110</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F52" s="1" t="str">
+        <f>DEC2HEX(B52+E52)</f>
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>19</v>
       </c>
       <c r="B53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>135</v>
       </c>
-      <c r="C53" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D53" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C53" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10000111</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F53" s="1" t="str">
+        <f>DEC2HEX(B53+E53)</f>
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>20</v>
       </c>
       <c r="B54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>136</v>
       </c>
-      <c r="C54" s="1">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C54" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001000</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="str">
+        <f>DEC2HEX(B54+E54)</f>
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>21</v>
       </c>
       <c r="B55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>137</v>
       </c>
-      <c r="C55" s="1">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C55" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001001</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1" t="str">
+        <f>DEC2HEX(B55+E55)</f>
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>22</v>
       </c>
       <c r="B56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>138</v>
       </c>
-      <c r="C56" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D56" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C56" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001010</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F56" s="1" t="str">
+        <f>DEC2HEX(B56+E56)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>23</v>
       </c>
       <c r="B57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>139</v>
       </c>
-      <c r="C57" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D57" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C57" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001011</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F57" s="1" t="str">
+        <f>DEC2HEX(B57+E57)</f>
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>24</v>
       </c>
       <c r="B58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="C58" s="1">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C58" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001100</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1" t="str">
+        <f>DEC2HEX(B58+E58)</f>
         <v>8C</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>25</v>
       </c>
       <c r="B59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>141</v>
       </c>
-      <c r="C59" s="1">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C59" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001101</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1" t="str">
+        <f>DEC2HEX(B59+E59)</f>
         <v>8D</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>26</v>
       </c>
       <c r="B60" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>142</v>
       </c>
-      <c r="C60" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D60" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C60" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001110</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F60" s="1" t="str">
+        <f>DEC2HEX(B60+E60)</f>
         <v>8A</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>27</v>
       </c>
       <c r="B61" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
-      <c r="C61" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D61" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C61" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10001111</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F61" s="1" t="str">
+        <f>DEC2HEX(B61+E61)</f>
         <v>8B</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>28</v>
       </c>
       <c r="B62" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
-      <c r="C62" s="1">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C62" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10010000</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1" t="str">
+        <f>DEC2HEX(B62+E62)</f>
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>29</v>
       </c>
       <c r="B63" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
-      <c r="C63" s="1">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C63" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10010001</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1" t="str">
+        <f>DEC2HEX(B63+E63)</f>
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>30</v>
       </c>
       <c r="B64" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
-      <c r="C64" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D64" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C64" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10010010</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F64" s="1" t="str">
+        <f>DEC2HEX(B64+E64)</f>
         <v>8E</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>31</v>
       </c>
       <c r="B65" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
-      <c r="C65" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D65" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="C65" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10010011</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="F65" s="1" t="str">
+        <f>DEC2HEX(B65+E65)</f>
         <v>8F</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>32</v>
       </c>
       <c r="B66" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
-      <c r="C66" s="1">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1" t="str">
-        <f t="shared" ref="D66:D97" si="4">DEC2HEX(B66+C66)</f>
+      <c r="C66" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10010100</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="1" t="str">
+        <f t="shared" ref="F66:F97" si="6">DEC2HEX(B66+E66)</f>
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>33</v>
       </c>
       <c r="B67" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>149</v>
       </c>
-      <c r="C67" s="1">
-        <v>0</v>
-      </c>
-      <c r="D67" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C67" s="1" t="str">
+        <f t="shared" ref="C67:C130" si="7">DEC2BIN(B67)</f>
+        <v>10010101</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D130" si="8">_xlfn.BITAND(C67, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" ref="E67:E130" si="9">D67*-2</f>
+        <v>0</v>
+      </c>
+      <c r="F67" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>34</v>
       </c>
       <c r="B68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="C68" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D68" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C68" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10010110</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E68" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F68" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>35</v>
       </c>
       <c r="B69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
-      <c r="C69" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D69" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C69" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10010111</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F69" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>36</v>
       </c>
       <c r="B70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>152</v>
       </c>
-      <c r="C70" s="1">
-        <v>0</v>
-      </c>
-      <c r="D70" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C70" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011000</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F70" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>37</v>
       </c>
       <c r="B71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
-      <c r="C71" s="1">
-        <v>0</v>
-      </c>
-      <c r="D71" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C71" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011001</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>38</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
-      <c r="C72" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D72" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C72" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011010</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F72" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>39</v>
       </c>
       <c r="B73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
-      <c r="C73" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D73" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C73" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011011</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F73" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>40</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>156</v>
       </c>
-      <c r="C74" s="1">
-        <v>0</v>
-      </c>
-      <c r="D74" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C74" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011100</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F74" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>9C</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>41</v>
       </c>
       <c r="B75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
-      <c r="C75" s="1">
-        <v>0</v>
-      </c>
-      <c r="D75" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C75" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011101</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F75" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>9D</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>42</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>158</v>
       </c>
-      <c r="C76" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D76" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C76" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011110</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E76" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F76" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>9A</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>43</v>
       </c>
       <c r="B77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
-      <c r="C77" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D77" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C77" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10011111</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F77" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>9B</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>44</v>
       </c>
       <c r="B78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
-      <c r="C78" s="1">
-        <v>0</v>
-      </c>
-      <c r="D78" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C78" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100000</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F78" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>45</v>
       </c>
       <c r="B79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
-      <c r="C79" s="1">
-        <v>0</v>
-      </c>
-      <c r="D79" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C79" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100001</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>46</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
-      <c r="C80" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D80" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C80" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100010</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E80" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F80" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>9E</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>47</v>
       </c>
       <c r="B81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
-      <c r="C81" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D81" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C81" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100011</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F81" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>9F</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>48</v>
       </c>
       <c r="B82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="C82" s="1">
-        <v>0</v>
-      </c>
-      <c r="D82" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C82" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100100</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E82" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F82" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>49</v>
       </c>
       <c r="B83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="C83" s="1">
-        <v>0</v>
-      </c>
-      <c r="D83" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C83" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100101</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>50</v>
       </c>
       <c r="B84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
-      <c r="C84" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D84" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C84" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100110</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E84" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F84" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>51</v>
       </c>
       <c r="B85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="C85" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D85" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C85" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10100111</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E85" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F85" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A3</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>52</v>
       </c>
       <c r="B86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
-      <c r="C86" s="1">
-        <v>0</v>
-      </c>
-      <c r="D86" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C86" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101000</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F86" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A8</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>53</v>
       </c>
       <c r="B87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
-      <c r="C87" s="1">
-        <v>0</v>
-      </c>
-      <c r="D87" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C87" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101001</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E87" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F87" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A9</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>54</v>
       </c>
       <c r="B88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
-      <c r="C88" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D88" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C88" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101010</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E88" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F88" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A6</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>55</v>
       </c>
       <c r="B89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
-      <c r="C89" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D89" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C89" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101011</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E89" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F89" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>A7</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>56</v>
       </c>
       <c r="B90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
-      <c r="C90" s="1">
-        <v>0</v>
-      </c>
-      <c r="D90" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C90" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101100</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E90" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F90" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>AC</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>57</v>
       </c>
       <c r="B91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
-      <c r="C91" s="1">
-        <v>0</v>
-      </c>
-      <c r="D91" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C91" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101101</v>
+      </c>
+      <c r="D91" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E91" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F91" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>AD</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>58</v>
       </c>
       <c r="B92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
-      <c r="C92" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D92" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C92" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101110</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E92" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F92" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>AA</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>59</v>
       </c>
       <c r="B93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
-      <c r="C93" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D93" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C93" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10101111</v>
+      </c>
+      <c r="D93" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E93" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F93" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>AB</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>60</v>
       </c>
       <c r="B94" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
-      <c r="C94" s="1">
-        <v>0</v>
-      </c>
-      <c r="D94" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C94" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110000</v>
+      </c>
+      <c r="D94" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E94" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F94" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>B0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>61</v>
       </c>
       <c r="B95" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
-      <c r="C95" s="1">
-        <v>0</v>
-      </c>
-      <c r="D95" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C95" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110001</v>
+      </c>
+      <c r="D95" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E95" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F95" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>B1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>62</v>
       </c>
       <c r="B96" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
-      <c r="C96" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D96" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C96" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110010</v>
+      </c>
+      <c r="D96" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E96" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F96" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>AE</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>63</v>
       </c>
       <c r="B97" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>179</v>
       </c>
-      <c r="C97" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D97" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="C97" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110011</v>
+      </c>
+      <c r="D97" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E97" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F97" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>AF</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>64</v>
       </c>
       <c r="B98" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
-      <c r="C98" s="1">
-        <v>0</v>
-      </c>
-      <c r="D98" s="1" t="str">
-        <f t="shared" ref="D98:D129" si="5">DEC2HEX(B98+C98)</f>
+      <c r="C98" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110100</v>
+      </c>
+      <c r="D98" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="1" t="str">
+        <f t="shared" ref="F98:F129" si="10">DEC2HEX(B98+E98)</f>
         <v>B4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>65</v>
       </c>
       <c r="B99" s="1">
-        <f t="shared" ref="B99:B133" si="6">116+A99</f>
+        <f t="shared" ref="B99:B133" si="11">116+A99</f>
         <v>181</v>
       </c>
-      <c r="C99" s="1">
-        <v>0</v>
-      </c>
-      <c r="D99" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C99" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110101</v>
+      </c>
+      <c r="D99" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B5</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>66</v>
       </c>
       <c r="B100" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>182</v>
       </c>
-      <c r="C100" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D100" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C100" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110110</v>
+      </c>
+      <c r="D100" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E100" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F100" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B2</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>67</v>
       </c>
       <c r="B101" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>183</v>
       </c>
-      <c r="C101" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D101" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C101" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10110111</v>
+      </c>
+      <c r="D101" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F101" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>68</v>
       </c>
       <c r="B102" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>184</v>
       </c>
-      <c r="C102" s="1">
-        <v>0</v>
-      </c>
-      <c r="D102" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C102" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111000</v>
+      </c>
+      <c r="D102" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E102" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F102" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B8</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>69</v>
       </c>
       <c r="B103" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>185</v>
       </c>
-      <c r="C103" s="1">
-        <v>0</v>
-      </c>
-      <c r="D103" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C103" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111001</v>
+      </c>
+      <c r="D103" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E103" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F103" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B9</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>70</v>
       </c>
       <c r="B104" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>186</v>
       </c>
-      <c r="C104" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D104" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C104" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111010</v>
+      </c>
+      <c r="D104" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E104" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F104" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B6</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>71</v>
       </c>
       <c r="B105" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>187</v>
       </c>
-      <c r="C105" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D105" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C105" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111011</v>
+      </c>
+      <c r="D105" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E105" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F105" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>B7</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>72</v>
       </c>
       <c r="B106" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>188</v>
       </c>
-      <c r="C106" s="1">
-        <v>0</v>
-      </c>
-      <c r="D106" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C106" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111100</v>
+      </c>
+      <c r="D106" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E106" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F106" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>BC</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>73</v>
       </c>
       <c r="B107" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>189</v>
       </c>
-      <c r="C107" s="1">
-        <v>0</v>
-      </c>
-      <c r="D107" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C107" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111101</v>
+      </c>
+      <c r="D107" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E107" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F107" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>BD</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>74</v>
       </c>
       <c r="B108" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>190</v>
       </c>
-      <c r="C108" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D108" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C108" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111110</v>
+      </c>
+      <c r="D108" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E108" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F108" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>BA</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>75</v>
       </c>
       <c r="B109" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>191</v>
       </c>
-      <c r="C109" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D109" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C109" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>10111111</v>
+      </c>
+      <c r="D109" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E109" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F109" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>BB</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>76</v>
       </c>
       <c r="B110" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>192</v>
       </c>
-      <c r="C110" s="1">
-        <v>0</v>
-      </c>
-      <c r="D110" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C110" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000000</v>
+      </c>
+      <c r="D110" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E110" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F110" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>77</v>
       </c>
       <c r="B111" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>193</v>
       </c>
-      <c r="C111" s="1">
-        <v>0</v>
-      </c>
-      <c r="D111" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C111" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000001</v>
+      </c>
+      <c r="D111" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E111" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F111" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>78</v>
       </c>
       <c r="B112" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>194</v>
       </c>
-      <c r="C112" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D112" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C112" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000010</v>
+      </c>
+      <c r="D112" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E112" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F112" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>BE</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>79</v>
       </c>
       <c r="B113" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>195</v>
       </c>
-      <c r="C113" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D113" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C113" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000011</v>
+      </c>
+      <c r="D113" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E113" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F113" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>BF</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>80</v>
       </c>
       <c r="B114" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>196</v>
       </c>
-      <c r="C114" s="1">
-        <v>0</v>
-      </c>
-      <c r="D114" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C114" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000100</v>
+      </c>
+      <c r="D114" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E114" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F114" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>81</v>
       </c>
       <c r="B115" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>197</v>
       </c>
-      <c r="C115" s="1">
-        <v>0</v>
-      </c>
-      <c r="D115" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C115" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000101</v>
+      </c>
+      <c r="D115" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E115" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F115" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C5</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>82</v>
       </c>
       <c r="B116" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>198</v>
       </c>
-      <c r="C116" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D116" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C116" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000110</v>
+      </c>
+      <c r="D116" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E116" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F116" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>83</v>
       </c>
       <c r="B117" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>199</v>
       </c>
-      <c r="C117" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D117" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C117" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11000111</v>
+      </c>
+      <c r="D117" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E117" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F117" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C3</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>84</v>
       </c>
       <c r="B118" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>200</v>
       </c>
-      <c r="C118" s="1">
-        <v>0</v>
-      </c>
-      <c r="D118" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C118" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001000</v>
+      </c>
+      <c r="D118" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E118" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C8</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>85</v>
       </c>
       <c r="B119" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>201</v>
       </c>
-      <c r="C119" s="1">
-        <v>0</v>
-      </c>
-      <c r="D119" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C119" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001001</v>
+      </c>
+      <c r="D119" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E119" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F119" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C9</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>86</v>
       </c>
       <c r="B120" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>202</v>
       </c>
-      <c r="C120" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D120" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C120" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001010</v>
+      </c>
+      <c r="D120" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E120" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F120" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C6</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>87</v>
       </c>
       <c r="B121" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>203</v>
       </c>
-      <c r="C121" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D121" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C121" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001011</v>
+      </c>
+      <c r="D121" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E121" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F121" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>C7</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>88</v>
       </c>
       <c r="B122" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>204</v>
       </c>
-      <c r="C122" s="1">
-        <v>0</v>
-      </c>
-      <c r="D122" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C122" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001100</v>
+      </c>
+      <c r="D122" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E122" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F122" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>CC</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>89</v>
       </c>
       <c r="B123" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>205</v>
       </c>
-      <c r="C123" s="1">
-        <v>0</v>
-      </c>
-      <c r="D123" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C123" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001101</v>
+      </c>
+      <c r="D123" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E123" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F123" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>CD</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>90</v>
       </c>
       <c r="B124" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>206</v>
       </c>
-      <c r="C124" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D124" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C124" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001110</v>
+      </c>
+      <c r="D124" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E124" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F124" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>CA</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>91</v>
       </c>
       <c r="B125" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>207</v>
       </c>
-      <c r="C125" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D125" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C125" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11001111</v>
+      </c>
+      <c r="D125" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E125" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F125" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>CB</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>92</v>
       </c>
       <c r="B126" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>208</v>
       </c>
-      <c r="C126" s="1">
-        <v>0</v>
-      </c>
-      <c r="D126" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C126" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11010000</v>
+      </c>
+      <c r="D126" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E126" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F126" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>D0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>93</v>
       </c>
       <c r="B127" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>209</v>
       </c>
-      <c r="C127" s="1">
-        <v>0</v>
-      </c>
-      <c r="D127" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C127" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11010001</v>
+      </c>
+      <c r="D127" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E127" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F127" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>D1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>94</v>
       </c>
       <c r="B128" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>210</v>
       </c>
-      <c r="C128" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D128" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C128" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11010010</v>
+      </c>
+      <c r="D128" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E128" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F128" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>CE</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>95</v>
       </c>
       <c r="B129" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>211</v>
       </c>
-      <c r="C129" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D129" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="C129" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11010011</v>
+      </c>
+      <c r="D129" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E129" s="1">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="F129" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>CF</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>96</v>
       </c>
       <c r="B130" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>212</v>
       </c>
-      <c r="C130" s="1">
-        <v>0</v>
-      </c>
-      <c r="D130" s="1" t="str">
-        <f t="shared" ref="D130:D161" si="7">DEC2HEX(B130+C130)</f>
+      <c r="C130" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>11010100</v>
+      </c>
+      <c r="D130" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E130" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F130" s="1" t="str">
+        <f t="shared" ref="F130:F133" si="12">DEC2HEX(B130+E130)</f>
         <v>D4</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>97</v>
       </c>
       <c r="B131" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>213</v>
       </c>
-      <c r="C131" s="1">
-        <v>0</v>
-      </c>
-      <c r="D131" s="1" t="str">
-        <f t="shared" si="7"/>
+      <c r="C131" s="1" t="str">
+        <f t="shared" ref="C131:C133" si="13">DEC2BIN(B131)</f>
+        <v>11010101</v>
+      </c>
+      <c r="D131" s="1">
+        <f t="shared" ref="D131:D133" si="14">_xlfn.BITAND(C131, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="E131" s="1">
+        <f t="shared" ref="E131:E133" si="15">D131*-2</f>
+        <v>0</v>
+      </c>
+      <c r="F131" s="1" t="str">
+        <f t="shared" si="12"/>
         <v>D5</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>98</v>
       </c>
       <c r="B132" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>214</v>
       </c>
-      <c r="C132" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D132" s="1" t="str">
-        <f t="shared" si="7"/>
+      <c r="C132" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>11010110</v>
+      </c>
+      <c r="D132" s="1">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="E132" s="1">
+        <f t="shared" si="15"/>
+        <v>-4</v>
+      </c>
+      <c r="F132" s="1" t="str">
+        <f t="shared" si="12"/>
         <v>D2</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>99</v>
       </c>
       <c r="B133" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>215</v>
       </c>
-      <c r="C133" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D133" s="1" t="str">
-        <f t="shared" si="7"/>
+      <c r="C133" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>11010111</v>
+      </c>
+      <c r="D133" s="1">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="E133" s="1">
+        <f t="shared" si="15"/>
+        <v>-4</v>
+      </c>
+      <c r="F133" s="1" t="str">
+        <f t="shared" si="12"/>
         <v>D3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>